<commit_message>
reduced number of climate zone polygons
</commit_message>
<xml_diff>
--- a/Build_Status.xlsx
+++ b/Build_Status.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB4D51E-7E6F-8648-B0CD-D14260471C7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6768401C-7468-604F-818C-F8D0D76C2D66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="2140" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{FFB251FF-B283-874E-B523-E9C965B2BDF7}"/>
+    <workbookView xWindow="3340" yWindow="460" windowWidth="27640" windowHeight="16940" xr2:uid="{FFB251FF-B283-874E-B523-E9C965B2BDF7}"/>
   </bookViews>
   <sheets>
     <sheet name="CD Status" sheetId="2" r:id="rId1"/>
     <sheet name="HUC_Status" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CD Status'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CD Status'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">HUC_Status!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>Alberta</t>
   </si>
@@ -82,9 +82,6 @@
     <t>New Mexico</t>
   </si>
   <si>
-    <t>Nevada</t>
-  </si>
-  <si>
     <t>Nebraska</t>
   </si>
   <si>
@@ -112,12 +109,6 @@
     <t>Colorado</t>
   </si>
   <si>
-    <t>California</t>
-  </si>
-  <si>
-    <t>British Columbia</t>
-  </si>
-  <si>
     <t>Wyoming</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>Utah</t>
   </si>
   <si>
-    <t>Texas</t>
-  </si>
-  <si>
     <t>Tennessee</t>
   </si>
   <si>
@@ -214,9 +202,6 @@
     <t>Powder-Tongue</t>
   </si>
   <si>
-    <t>graupel</t>
-  </si>
-  <si>
     <t>Lower Yellowstone</t>
   </si>
   <si>
@@ -269,13 +254,19 @@
   </si>
   <si>
     <t>sundog</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>7,8,9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -345,6 +336,27 @@
       <b/>
       <sz val="14"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -438,7 +450,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -479,10 +491,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -504,6 +512,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -532,7 +549,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6667500" cy="2882900"/>
@@ -1105,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5EA337-0194-1549-96B3-842E71A29D75}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C24"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1120,40 +1137,43 @@
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="13">
-        <v>3200</v>
+        <v>500</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C2" s="13">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D2" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="13">
-        <v>3400</v>
+        <v>3200</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="13">
         <v>9</v>
@@ -1162,54 +1182,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="13">
-        <v>3900</v>
+        <v>3400</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="13">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="13">
-        <v>4000</v>
+        <v>3900</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="13">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D5" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="13">
-        <v>4100</v>
+        <v>4000</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C6" s="13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D6" s="12">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="13">
         <v>4200</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C7" s="13">
         <v>7</v>
@@ -1218,12 +1238,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="13">
         <v>4700</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="13">
         <v>9</v>
@@ -1232,12 +1252,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="13">
         <v>4800</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C9" s="13">
         <v>10</v>
@@ -1246,325 +1266,717 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="13">
-        <v>80000</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="13">
+    <row r="10" spans="1:5">
+      <c r="A10" s="11">
+        <v>40000</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="11">
+        <v>9</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9">
+        <v>2000</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="D10" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="13">
-        <v>400</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="13">
+      <c r="D11" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9">
+        <v>2100</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="9">
+        <v>9</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="9">
+        <v>2200</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="13">
-        <v>500</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="13">
-        <v>9</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="11">
-        <v>40000</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="11">
+      <c r="D13" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="9">
+        <v>2300</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="9">
-        <v>2000</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="C14" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="9">
-        <v>2100</v>
+        <v>2400</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C15" s="9">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="9">
-        <v>2200</v>
+        <v>2500</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C16" s="9">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:13">
       <c r="A17" s="9">
-        <v>2300</v>
+        <v>2900</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C17" s="9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="9">
-        <v>2400</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="9">
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33"/>
+      <c r="K17" s="33"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="7">
+        <v>100</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="33"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="7">
+        <v>200</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="7">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" s="33"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="7">
+        <v>300</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="7">
+        <v>6</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="33"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="5">
+        <v>3</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="33"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="5">
+        <v>1100</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="9">
-        <v>2500</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="9">
-        <v>8</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="9">
-        <v>2600</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="C22" s="5">
+        <v>9</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="33"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="33"/>
+      <c r="L22" s="33"/>
+      <c r="M22" s="33"/>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="5">
+        <v>1200</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="G23" s="33"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="33"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
+      <c r="L23" s="33"/>
+      <c r="M23" s="33"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="5">
+        <v>1300</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5">
+        <v>9</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="33"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="5">
+        <v>1400</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
+      <c r="M25" s="33"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="5">
+        <v>1500</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="4"/>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
+      <c r="G26" s="33"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="33"/>
+      <c r="J26" s="33"/>
+      <c r="K26" s="33"/>
+      <c r="L26" s="33"/>
+      <c r="M26" s="33"/>
+    </row>
+    <row r="27" spans="1:13">
+      <c r="A27" s="3">
+        <v>50000</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="3">
+        <v>18</v>
+      </c>
+      <c r="G27" s="33"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+    </row>
+    <row r="28" spans="1:13">
+      <c r="A28" s="3">
+        <v>60000</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
         <v>14</v>
       </c>
-      <c r="C20" s="9">
-        <v>3</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="9">
-        <v>2900</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="9">
+      <c r="G28" s="33"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+    </row>
+    <row r="29" spans="1:13" s="2" customFormat="1">
+      <c r="A29" s="3">
+        <v>70000</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
         <v>7</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="7">
-        <v>100</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="7">
-        <v>4</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7">
-        <v>200</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="7">
-        <v>6</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="7">
-        <v>300</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="7">
-        <v>9</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="5">
-        <v>1000</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="5">
-        <v>6</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="5">
-        <v>1100</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26" s="5">
-        <v>9</v>
-      </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="5">
-        <v>1200</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="5">
-        <v>6</v>
-      </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="5">
-        <v>1300</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" s="5">
-        <v>9</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="5">
-        <v>1400</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="5">
-        <v>9</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="5">
-        <v>1500</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="5">
-        <v>2</v>
-      </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="3">
-        <v>50000</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31" s="3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="3">
-        <v>60000</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" s="2" customFormat="1">
-      <c r="A33" s="3">
-        <v>70000</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="3">
-        <v>14</v>
-      </c>
+      <c r="G29" s="35"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="35"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="35"/>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="G30" s="33"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="G31" s="33"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="G32" s="33"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+    </row>
+    <row r="33" spans="7:13">
+      <c r="G33" s="33"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+    </row>
+    <row r="34" spans="7:13">
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+    </row>
+    <row r="35" spans="7:13">
+      <c r="G35" s="33"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+    </row>
+    <row r="36" spans="7:13">
+      <c r="G36" s="33"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+    </row>
+    <row r="37" spans="7:13">
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+    </row>
+    <row r="38" spans="7:13">
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+    </row>
+    <row r="39" spans="7:13">
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="33"/>
+    </row>
+    <row r="40" spans="7:13">
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="33"/>
+    </row>
+    <row r="41" spans="7:13">
+      <c r="G41" s="33"/>
+      <c r="H41" s="33"/>
+      <c r="I41" s="33"/>
+      <c r="J41" s="33"/>
+      <c r="K41" s="33"/>
+      <c r="L41" s="33"/>
+      <c r="M41" s="33"/>
+    </row>
+    <row r="42" spans="7:13">
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+    </row>
+    <row r="43" spans="7:13">
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33"/>
+      <c r="K43" s="33"/>
+      <c r="L43" s="33"/>
+      <c r="M43" s="33"/>
+    </row>
+    <row r="44" spans="7:13">
+      <c r="G44" s="33"/>
+      <c r="H44" s="33"/>
+      <c r="I44" s="33"/>
+      <c r="J44" s="33"/>
+      <c r="K44" s="33"/>
+      <c r="L44" s="33"/>
+      <c r="M44" s="33"/>
+    </row>
+    <row r="45" spans="7:13">
+      <c r="G45" s="33"/>
+      <c r="H45" s="33"/>
+      <c r="I45" s="33"/>
+      <c r="J45" s="33"/>
+      <c r="K45" s="33"/>
+      <c r="L45" s="33"/>
+      <c r="M45" s="33"/>
+    </row>
+    <row r="46" spans="7:13">
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33"/>
+      <c r="K46" s="33"/>
+      <c r="L46" s="33"/>
+      <c r="M46" s="33"/>
+    </row>
+    <row r="47" spans="7:13">
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+    </row>
+    <row r="48" spans="7:13">
+      <c r="G48" s="33"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="33"/>
+      <c r="J48" s="33"/>
+      <c r="K48" s="33"/>
+      <c r="L48" s="33"/>
+      <c r="M48" s="33"/>
+    </row>
+    <row r="49" spans="7:13">
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33"/>
+      <c r="K49" s="33"/>
+      <c r="L49" s="33"/>
+      <c r="M49" s="33"/>
+    </row>
+    <row r="50" spans="7:13">
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33"/>
+      <c r="K50" s="33"/>
+      <c r="L50" s="33"/>
+      <c r="M50" s="33"/>
+    </row>
+    <row r="51" spans="7:13">
+      <c r="G51" s="33"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="33"/>
+      <c r="J51" s="33"/>
+      <c r="K51" s="33"/>
+      <c r="L51" s="33"/>
+      <c r="M51" s="33"/>
+    </row>
+    <row r="52" spans="7:13">
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="33"/>
+      <c r="M52" s="33"/>
+    </row>
+    <row r="53" spans="7:13">
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
+      <c r="K53" s="33"/>
+      <c r="L53" s="33"/>
+      <c r="M53" s="33"/>
+    </row>
+    <row r="54" spans="7:13">
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
+      <c r="L54" s="33"/>
+      <c r="M54" s="33"/>
+    </row>
+    <row r="55" spans="7:13">
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="33"/>
+      <c r="K55" s="33"/>
+      <c r="L55" s="33"/>
+      <c r="M55" s="33"/>
+    </row>
+    <row r="56" spans="7:13">
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+    </row>
+    <row r="57" spans="7:13">
+      <c r="G57" s="33"/>
+      <c r="H57" s="33"/>
+      <c r="I57" s="33"/>
+      <c r="J57" s="33"/>
+      <c r="K57" s="33"/>
+      <c r="L57" s="33"/>
+      <c r="M57" s="33"/>
+    </row>
+    <row r="58" spans="7:13">
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="33"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="33"/>
+      <c r="L58" s="33"/>
+      <c r="M58" s="33"/>
+    </row>
+    <row r="59" spans="7:13">
+      <c r="G59" s="33"/>
+      <c r="H59" s="33"/>
+      <c r="I59" s="33"/>
+      <c r="J59" s="33"/>
+      <c r="K59" s="33"/>
+      <c r="L59" s="33"/>
+      <c r="M59" s="33"/>
+    </row>
+    <row r="60" spans="7:13">
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="33"/>
+      <c r="K60" s="33"/>
+      <c r="L60" s="33"/>
+      <c r="M60" s="33"/>
+    </row>
+    <row r="61" spans="7:13">
+      <c r="G61" s="33"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+    </row>
+    <row r="62" spans="7:13">
+      <c r="G62" s="33"/>
+      <c r="H62" s="33"/>
+      <c r="I62" s="33"/>
+      <c r="J62" s="33"/>
+      <c r="K62" s="33"/>
+      <c r="L62" s="33"/>
+      <c r="M62" s="33"/>
+    </row>
+    <row r="63" spans="7:13">
+      <c r="G63" s="33"/>
+      <c r="H63" s="33"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="33"/>
+      <c r="K63" s="33"/>
+      <c r="L63" s="33"/>
+      <c r="M63" s="33"/>
+    </row>
+    <row r="64" spans="7:13">
+      <c r="G64" s="33"/>
+      <c r="H64" s="33"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="33"/>
+      <c r="M64" s="33"/>
+    </row>
+    <row r="65" spans="7:13">
+      <c r="G65" s="33"/>
+      <c r="H65" s="33"/>
+      <c r="I65" s="33"/>
+      <c r="J65" s="33"/>
+      <c r="K65" s="33"/>
+      <c r="L65" s="33"/>
+      <c r="M65" s="33"/>
+    </row>
+    <row r="66" spans="7:13">
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33"/>
+      <c r="K66" s="33"/>
+      <c r="L66" s="33"/>
+      <c r="M66" s="33"/>
+    </row>
+    <row r="67" spans="7:13">
+      <c r="G67" s="33"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="33"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="33"/>
+      <c r="L67" s="33"/>
+      <c r="M67" s="33"/>
+    </row>
+    <row r="68" spans="7:13">
+      <c r="G68" s="33"/>
+      <c r="H68" s="33"/>
+      <c r="I68" s="33"/>
+      <c r="J68" s="33"/>
+      <c r="K68" s="33"/>
+      <c r="L68" s="33"/>
+      <c r="M68" s="33"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1" xr:uid="{A3CC9153-DA2A-9649-A26A-D3C1B1D4FEE8}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
-      <sortCondition ref="D1:D33"/>
+  <autoFilter ref="A1:M1" xr:uid="{1080914A-907F-7B4C-8207-1C600B07CD6A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M29">
+      <sortCondition ref="D1:D29"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1576,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D7117F-F167-164D-9162-D99D52066453}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1591,223 +2003,223 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="B1" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>34</v>
+      <c r="A1" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>30</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="29">
+      <c r="A2" s="27">
         <v>1002</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="27">
         <v>8</v>
       </c>
-      <c r="C2" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="28">
+      <c r="C2" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="26">
         <v>0</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="29">
+      <c r="A3" s="27">
         <v>1003</v>
       </c>
-      <c r="B3" s="29">
+      <c r="B3" s="27">
         <v>10</v>
       </c>
-      <c r="C3" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="28">
+      <c r="C3" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="26">
         <v>0</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="29">
+      <c r="A4" s="27">
         <v>1012</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="27">
         <v>16</v>
       </c>
-      <c r="C4" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="28">
+      <c r="C4" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="29">
+      <c r="A5" s="27">
         <v>1016</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="27">
         <v>10</v>
       </c>
-      <c r="C5" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="28">
+      <c r="C5" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="29">
+      <c r="A6" s="27">
         <v>1017</v>
       </c>
-      <c r="B6" s="29">
+      <c r="B6" s="27">
         <v>7</v>
       </c>
-      <c r="C6" s="29" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="28">
+      <c r="C6" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="29">
+      <c r="A7" s="27">
         <v>1004</v>
       </c>
-      <c r="B7" s="29">
+      <c r="B7" s="27">
         <v>11</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="28">
+      <c r="C7" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="29">
+      <c r="A8" s="27">
         <v>1015</v>
       </c>
-      <c r="B8" s="29">
+      <c r="B8" s="27">
         <v>7</v>
       </c>
-      <c r="C8" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="30">
+      <c r="C8" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="28">
         <v>0</v>
       </c>
       <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="31">
+      <c r="A9" s="29">
         <v>1014</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="29">
         <v>9</v>
       </c>
-      <c r="C9" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="30">
+      <c r="C9" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="28">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="29">
+      <c r="A10" s="27">
         <v>1013</v>
       </c>
-      <c r="B10" s="29">
+      <c r="B10" s="27">
         <v>18</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="28">
+      <c r="C10" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="25">
+      <c r="A11" s="36">
+        <v>1010</v>
+      </c>
+      <c r="B11" s="36">
+        <v>5</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="23">
         <v>1006</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B12" s="23">
         <v>7</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="27">
-        <v>1010</v>
-      </c>
-      <c r="B12" s="27">
-        <v>5</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>58</v>
+      <c r="C12" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="27">
+      <c r="A13" s="25">
         <v>1009</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="25">
         <v>12</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>56</v>
+      <c r="C13" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="25">
+      <c r="A14" s="23">
         <v>1007</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="23">
         <v>8</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>54</v>
+      <c r="C14" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="21" customFormat="1">
-      <c r="A15" s="23">
+      <c r="A15" s="25">
         <v>1011</v>
       </c>
-      <c r="B15" s="23">
+      <c r="B15" s="25">
         <v>7</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>52</v>
+      <c r="C15" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>48</v>
       </c>
       <c r="E15" s="16"/>
     </row>
@@ -1819,7 +2231,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D16" s="19"/>
     </row>
@@ -1831,7 +2243,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D17" s="19"/>
     </row>
@@ -1843,7 +2255,7 @@
         <v>14</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D18" s="19"/>
     </row>
@@ -1855,7 +2267,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D19" s="19"/>
     </row>
@@ -1867,7 +2279,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D20" s="19"/>
     </row>
@@ -1879,7 +2291,7 @@
         <v>10</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D21" s="19"/>
       <c r="H21" s="16">
@@ -1895,7 +2307,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D22" s="19"/>
     </row>
@@ -1907,7 +2319,7 @@
         <v>7</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D23" s="19"/>
     </row>
@@ -1919,7 +2331,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D24" s="19"/>
     </row>
@@ -1931,7 +2343,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D25" s="19"/>
     </row>
@@ -1943,7 +2355,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D26" s="19"/>
     </row>
@@ -1967,7 +2379,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D28" s="19"/>
     </row>
@@ -1979,7 +2391,7 @@
         <v>14</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D29" s="19"/>
     </row>
@@ -1991,7 +2403,7 @@
         <v>5</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D30" s="19"/>
     </row>

</xml_diff>

<commit_message>
fixing extreme huc analysis script
</commit_message>
<xml_diff>
--- a/Build_Status.xlsx
+++ b/Build_Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDC6B48-DB4A-9D45-AA85-9A862AC98CD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144F2DBD-AA0C-DD45-8486-631FA7C278FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14900" yWindow="460" windowWidth="33600" windowHeight="19600" activeTab="1" xr2:uid="{FFB251FF-B283-874E-B523-E9C965B2BDF7}"/>
+    <workbookView xWindow="1300" yWindow="1340" windowWidth="22460" windowHeight="17320" xr2:uid="{FFB251FF-B283-874E-B523-E9C965B2BDF7}"/>
   </bookViews>
   <sheets>
     <sheet name="CD Status" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t>Alberta</t>
   </si>
@@ -254,40 +254,40 @@
     <t>Sundog</t>
   </si>
   <si>
-    <t>nish-9-13</t>
-  </si>
-  <si>
     <t>Mist</t>
   </si>
   <si>
     <t>Graupel</t>
   </si>
   <si>
-    <t>Kansas 1-3</t>
-  </si>
-  <si>
-    <t>sundog Mist</t>
-  </si>
-  <si>
-    <t>Mist Graupel</t>
-  </si>
-  <si>
-    <t>Kansas 4-11</t>
-  </si>
-  <si>
     <t>bora</t>
   </si>
   <si>
-    <t>LowerMo</t>
-  </si>
-  <si>
-    <t>NebraskaCD</t>
-  </si>
-  <si>
-    <t>maelstrom</t>
-  </si>
-  <si>
-    <t>Miss Little Suoux</t>
+    <t>sundog</t>
+  </si>
+  <si>
+    <t>alabama</t>
+  </si>
+  <si>
+    <t>indiANA</t>
+  </si>
+  <si>
+    <t>qrk</t>
+  </si>
+  <si>
+    <t>Mississipi</t>
+  </si>
+  <si>
+    <t>suestafdsa</t>
+  </si>
+  <si>
+    <t>suestada   bora</t>
+  </si>
+  <si>
+    <t>mist</t>
+  </si>
+  <si>
+    <t>mist graupel maelstrom</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,12 +433,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,10 +563,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -615,12 +605,16 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -649,7 +643,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6667500" cy="2882900"/>
@@ -1224,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5EA337-0194-1549-96B3-842E71A29D75}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -1255,373 +1249,389 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="5">
-        <v>100</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
+      <c r="A2" s="7">
+        <v>500</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="7">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="5">
-        <v>300</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5">
-        <v>6</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
+      <c r="A3" s="7">
+        <v>1000</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="7">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C4" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" s="6">
         <v>0</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="7">
-        <v>1000</v>
+        <v>2900</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C5" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D5" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="24">
-        <v>1100</v>
-      </c>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="7">
+        <v>3200</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="7">
+        <v>3400</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7">
         <v>7</v>
       </c>
-      <c r="C6" s="24">
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="7">
+        <v>3900</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="7">
         <v>9</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="42">
-        <v>1200</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="42">
-        <v>3</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="21"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="24">
-        <v>1300</v>
-      </c>
-      <c r="B8" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="24">
-        <v>9</v>
-      </c>
-      <c r="D8" s="25"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="26">
-        <v>1400</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="26">
-        <v>9</v>
-      </c>
-      <c r="D9" s="27"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21"/>
+      <c r="A9" s="7">
+        <v>4000</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="7">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="7">
-        <v>1500</v>
+        <v>4200</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="7">
+        <v>7</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="7">
+        <v>4700</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7">
+        <v>9</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="7">
+        <v>4800</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="40">
+        <v>1200</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="40">
         <v>3</v>
       </c>
-      <c r="C10" s="7">
+      <c r="D13" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="42">
+        <v>2000</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="42">
         <v>1</v>
       </c>
-      <c r="D10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="46">
-        <v>2000</v>
-      </c>
-      <c r="B11" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="46">
+      <c r="D14" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="42">
+        <v>2200</v>
+      </c>
+      <c r="B15" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="42">
         <v>1</v>
       </c>
-      <c r="D11" s="47"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
-      <c r="M11" s="21"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="46">
-        <v>2100</v>
-      </c>
-      <c r="B12" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="46">
-        <v>9</v>
-      </c>
-      <c r="D12" s="47"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="46">
-        <v>2200</v>
-      </c>
-      <c r="B13" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="46">
+      <c r="D15" s="43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="5">
+        <v>100</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="5">
         <v>1</v>
       </c>
-      <c r="D13" s="47"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="46">
-        <v>2300</v>
-      </c>
-      <c r="B14" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="46">
-        <v>6</v>
-      </c>
-      <c r="D14" s="47"/>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" s="46">
-        <v>2400</v>
-      </c>
-      <c r="B15" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="46">
-        <v>6</v>
-      </c>
-      <c r="D15" s="47"/>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" s="42">
-        <v>2500</v>
-      </c>
-      <c r="B16" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="42">
-        <v>8</v>
-      </c>
-      <c r="D16" s="43"/>
+      <c r="D16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="5">
-        <v>2900</v>
+        <v>300</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C17" s="5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="22">
+        <v>1100</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="22">
+        <v>9</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="22">
+        <v>1300</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="22">
+        <v>9</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="24">
+        <v>1400</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="24">
+        <v>9</v>
+      </c>
+      <c r="D20" s="25"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="42">
+        <v>2100</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="42">
+        <v>9</v>
+      </c>
+      <c r="D21" s="43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="42">
+        <v>2300</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="42">
+        <v>6</v>
+      </c>
+      <c r="D22" s="43" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="7">
-        <v>3200</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="7">
-        <v>9</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" s="7">
-        <v>3400</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="7">
-        <v>7</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" s="7">
-        <v>3900</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="7">
-        <v>9</v>
-      </c>
-      <c r="D20" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" s="7">
-        <v>4000</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="7">
-        <v>1</v>
-      </c>
-      <c r="D21" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" s="7">
-        <v>4200</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="7">
-        <v>7</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0</v>
-      </c>
-    </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="7">
-        <v>4700</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" s="7">
-        <v>9</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0</v>
+      <c r="A23" s="42">
+        <v>2400</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="42">
+        <v>6</v>
+      </c>
+      <c r="D23" s="43" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="7">
-        <v>4800</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="7">
-        <v>10</v>
-      </c>
-      <c r="D24" s="6">
-        <v>0</v>
+      <c r="A24" s="40">
+        <v>2500</v>
+      </c>
+      <c r="B24" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="40">
+        <v>8</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1637,54 +1647,54 @@
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="24">
+      <c r="A26" s="22">
         <v>50000</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="24">
+      <c r="C26" s="22">
         <v>18</v>
       </c>
-      <c r="D26" s="25"/>
+      <c r="D26" s="23"/>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="24">
+      <c r="A27" s="22">
         <v>60000</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="24">
+      <c r="C27" s="22">
         <v>14</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
+      <c r="D27" s="23"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="24">
+      <c r="A28" s="22">
         <v>70000</v>
       </c>
-      <c r="B28" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="24">
+      <c r="B28" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="22">
         <v>7</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="21"/>
-      <c r="M28" s="21"/>
+      <c r="D28" s="23"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
     </row>
     <row r="29" spans="1:13" s="2" customFormat="1">
       <c r="A29" s="3"/>
@@ -1694,369 +1704,369 @@
         <f>D18</f>
         <v>0</v>
       </c>
-      <c r="G29" s="23"/>
-      <c r="H29" s="22"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="21"/>
-      <c r="M30" s="21"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="G31" s="21"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="G32" s="21"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="21"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="21"/>
-      <c r="L32" s="21"/>
-      <c r="M32" s="21"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
     </row>
     <row r="33" spans="7:13">
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
     </row>
     <row r="34" spans="7:13">
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="21"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
     </row>
     <row r="35" spans="7:13">
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="21"/>
-      <c r="L35" s="21"/>
-      <c r="M35" s="21"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
     </row>
     <row r="36" spans="7:13">
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="21"/>
-      <c r="L36" s="21"/>
-      <c r="M36" s="21"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
     </row>
     <row r="37" spans="7:13">
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
     </row>
     <row r="38" spans="7:13">
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="21"/>
-      <c r="L38" s="21"/>
-      <c r="M38" s="21"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
     </row>
     <row r="39" spans="7:13">
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="21"/>
-      <c r="L39" s="21"/>
-      <c r="M39" s="21"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
     </row>
     <row r="40" spans="7:13">
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="21"/>
-      <c r="L40" s="21"/>
-      <c r="M40" s="21"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
     </row>
     <row r="41" spans="7:13">
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="21"/>
-      <c r="L41" s="21"/>
-      <c r="M41" s="21"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
     </row>
     <row r="42" spans="7:13">
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="21"/>
-      <c r="L42" s="21"/>
-      <c r="M42" s="21"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
     </row>
     <row r="43" spans="7:13">
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="21"/>
-      <c r="L43" s="21"/>
-      <c r="M43" s="21"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
     </row>
     <row r="44" spans="7:13">
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="21"/>
-      <c r="L44" s="21"/>
-      <c r="M44" s="21"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
     </row>
     <row r="45" spans="7:13">
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="21"/>
-      <c r="L45" s="21"/>
-      <c r="M45" s="21"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
     </row>
     <row r="46" spans="7:13">
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="21"/>
-      <c r="L46" s="21"/>
-      <c r="M46" s="21"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
     </row>
     <row r="47" spans="7:13">
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="21"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
     </row>
     <row r="48" spans="7:13">
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="21"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="21"/>
-      <c r="M48" s="21"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+      <c r="K48" s="19"/>
+      <c r="L48" s="19"/>
+      <c r="M48" s="19"/>
     </row>
     <row r="49" spans="7:13">
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
-      <c r="K49" s="21"/>
-      <c r="L49" s="21"/>
-      <c r="M49" s="21"/>
+      <c r="G49" s="19"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="19"/>
+      <c r="K49" s="19"/>
+      <c r="L49" s="19"/>
+      <c r="M49" s="19"/>
     </row>
     <row r="50" spans="7:13">
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21"/>
-      <c r="M50" s="21"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
     </row>
     <row r="51" spans="7:13">
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="21"/>
-      <c r="K51" s="21"/>
-      <c r="L51" s="21"/>
-      <c r="M51" s="21"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="19"/>
+      <c r="K51" s="19"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="19"/>
     </row>
     <row r="52" spans="7:13">
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
-      <c r="K52" s="21"/>
-      <c r="L52" s="21"/>
-      <c r="M52" s="21"/>
+      <c r="G52" s="19"/>
+      <c r="H52" s="19"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="19"/>
+      <c r="K52" s="19"/>
+      <c r="L52" s="19"/>
+      <c r="M52" s="19"/>
     </row>
     <row r="53" spans="7:13">
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="21"/>
-      <c r="K53" s="21"/>
-      <c r="L53" s="21"/>
-      <c r="M53" s="21"/>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="19"/>
+      <c r="K53" s="19"/>
+      <c r="L53" s="19"/>
+      <c r="M53" s="19"/>
     </row>
     <row r="54" spans="7:13">
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="21"/>
-      <c r="K54" s="21"/>
-      <c r="L54" s="21"/>
-      <c r="M54" s="21"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="19"/>
+      <c r="K54" s="19"/>
+      <c r="L54" s="19"/>
+      <c r="M54" s="19"/>
     </row>
     <row r="55" spans="7:13">
-      <c r="G55" s="21"/>
-      <c r="H55" s="21"/>
-      <c r="I55" s="21"/>
-      <c r="J55" s="21"/>
-      <c r="K55" s="21"/>
-      <c r="L55" s="21"/>
-      <c r="M55" s="21"/>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="19"/>
+      <c r="L55" s="19"/>
+      <c r="M55" s="19"/>
     </row>
     <row r="56" spans="7:13">
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="21"/>
-      <c r="K56" s="21"/>
-      <c r="L56" s="21"/>
-      <c r="M56" s="21"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="19"/>
+      <c r="K56" s="19"/>
+      <c r="L56" s="19"/>
+      <c r="M56" s="19"/>
     </row>
     <row r="57" spans="7:13">
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="21"/>
-      <c r="K57" s="21"/>
-      <c r="L57" s="21"/>
-      <c r="M57" s="21"/>
+      <c r="G57" s="19"/>
+      <c r="H57" s="19"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="19"/>
+      <c r="K57" s="19"/>
+      <c r="L57" s="19"/>
+      <c r="M57" s="19"/>
     </row>
     <row r="58" spans="7:13">
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
-      <c r="L58" s="21"/>
-      <c r="M58" s="21"/>
+      <c r="G58" s="19"/>
+      <c r="H58" s="19"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="19"/>
+      <c r="K58" s="19"/>
+      <c r="L58" s="19"/>
+      <c r="M58" s="19"/>
     </row>
     <row r="59" spans="7:13">
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="21"/>
-      <c r="K59" s="21"/>
-      <c r="L59" s="21"/>
-      <c r="M59" s="21"/>
+      <c r="G59" s="19"/>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="19"/>
+      <c r="K59" s="19"/>
+      <c r="L59" s="19"/>
+      <c r="M59" s="19"/>
     </row>
     <row r="60" spans="7:13">
-      <c r="G60" s="21"/>
-      <c r="H60" s="21"/>
-      <c r="I60" s="21"/>
-      <c r="J60" s="21"/>
-      <c r="K60" s="21"/>
-      <c r="L60" s="21"/>
-      <c r="M60" s="21"/>
+      <c r="G60" s="19"/>
+      <c r="H60" s="19"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="19"/>
+      <c r="K60" s="19"/>
+      <c r="L60" s="19"/>
+      <c r="M60" s="19"/>
     </row>
     <row r="61" spans="7:13">
-      <c r="G61" s="21"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="21"/>
-      <c r="J61" s="21"/>
-      <c r="K61" s="21"/>
-      <c r="L61" s="21"/>
-      <c r="M61" s="21"/>
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="19"/>
+      <c r="K61" s="19"/>
+      <c r="L61" s="19"/>
+      <c r="M61" s="19"/>
     </row>
     <row r="62" spans="7:13">
-      <c r="G62" s="21"/>
-      <c r="H62" s="21"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="21"/>
-      <c r="M62" s="21"/>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="19"/>
+      <c r="K62" s="19"/>
+      <c r="L62" s="19"/>
+      <c r="M62" s="19"/>
     </row>
     <row r="63" spans="7:13">
-      <c r="G63" s="21"/>
-      <c r="H63" s="21"/>
-      <c r="I63" s="21"/>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
-      <c r="L63" s="21"/>
-      <c r="M63" s="21"/>
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="19"/>
+      <c r="K63" s="19"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
     </row>
     <row r="64" spans="7:13">
-      <c r="G64" s="21"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="21"/>
-      <c r="J64" s="21"/>
-      <c r="K64" s="21"/>
-      <c r="L64" s="21"/>
-      <c r="M64" s="21"/>
+      <c r="G64" s="19"/>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="19"/>
+      <c r="K64" s="19"/>
+      <c r="L64" s="19"/>
+      <c r="M64" s="19"/>
     </row>
     <row r="65" spans="7:13">
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
-      <c r="I65" s="21"/>
-      <c r="J65" s="21"/>
-      <c r="K65" s="21"/>
-      <c r="L65" s="21"/>
-      <c r="M65" s="21"/>
+      <c r="G65" s="19"/>
+      <c r="H65" s="19"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="19"/>
+      <c r="K65" s="19"/>
+      <c r="L65" s="19"/>
+      <c r="M65" s="19"/>
     </row>
     <row r="66" spans="7:13">
-      <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
-      <c r="L66" s="21"/>
-      <c r="M66" s="21"/>
+      <c r="G66" s="19"/>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="19"/>
+      <c r="K66" s="19"/>
+      <c r="L66" s="19"/>
+      <c r="M66" s="19"/>
     </row>
     <row r="67" spans="7:13">
-      <c r="G67" s="21"/>
-      <c r="H67" s="21"/>
-      <c r="I67" s="21"/>
-      <c r="J67" s="21"/>
-      <c r="K67" s="21"/>
-      <c r="L67" s="21"/>
-      <c r="M67" s="21"/>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="19"/>
+      <c r="K67" s="19"/>
+      <c r="L67" s="19"/>
+      <c r="M67" s="19"/>
     </row>
     <row r="68" spans="7:13">
-      <c r="G68" s="21"/>
-      <c r="H68" s="21"/>
-      <c r="I68" s="21"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="21"/>
-      <c r="L68" s="21"/>
-      <c r="M68" s="21"/>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="19"/>
+      <c r="K68" s="19"/>
+      <c r="L68" s="19"/>
+      <c r="M68" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:M1" xr:uid="{1080914A-907F-7B4C-8207-1C600B07CD6A}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M29">
-      <sortCondition ref="A1:A29"/>
+      <sortCondition ref="D1:D29"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2068,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D7117F-F167-164D-9162-D99D52066453}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -2083,16 +2093,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>29</v>
       </c>
       <c r="E1" s="12" t="s">
@@ -2100,16 +2110,16 @@
       </c>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="28">
+      <c r="A2" s="26">
         <v>1002</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="26">
         <v>8</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="27">
         <v>0</v>
       </c>
       <c r="E2" s="10" t="s">
@@ -2120,16 +2130,16 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="31">
+      <c r="A3" s="29">
         <v>1003</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="29">
         <v>10</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="30">
         <v>0</v>
       </c>
       <c r="E3" s="10" t="s">
@@ -2137,129 +2147,129 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="28">
+      <c r="A4" s="26">
         <v>1004</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="26">
         <v>11</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D4" s="29">
+      <c r="D4" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="28">
+      <c r="A5" s="26">
         <v>1006</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B5" s="26">
         <v>7</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="28">
+      <c r="A6" s="26">
         <v>1009</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="26">
         <v>11</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="28">
+      <c r="A7" s="26">
         <v>1010</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="26">
         <v>5</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="28">
+      <c r="A8" s="26">
         <v>1012</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="26">
         <v>16</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="29">
+      <c r="D8" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="28">
+      <c r="A9" s="26">
         <v>1013</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="26">
         <v>18</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="31">
+      <c r="A10" s="29">
         <v>1014</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="29">
         <v>9</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="30">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="28">
+      <c r="A11" s="26">
         <v>1015</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B11" s="26">
         <v>7</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="30">
         <v>0</v>
       </c>
       <c r="E11" s="15"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="28">
+      <c r="A12" s="26">
         <v>1016</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B12" s="26">
         <v>10</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="27">
         <v>0</v>
       </c>
       <c r="O12" s="10">
@@ -2268,16 +2278,16 @@
       </c>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="28">
+      <c r="A13" s="26">
         <v>1017</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B13" s="26">
         <v>7</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D13" s="29">
+      <c r="D13" s="27">
         <v>0</v>
       </c>
       <c r="O13" s="10">
@@ -2286,354 +2296,333 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="20" thickBot="1">
-      <c r="A14" s="28">
+      <c r="A14" s="26">
         <v>1020</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B14" s="26">
         <v>6</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="29">
+      <c r="D14" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="15" customFormat="1">
-      <c r="A15" s="28">
+      <c r="A15" s="26">
         <v>1021</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="26">
         <v>10</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="29">
+      <c r="D15" s="27">
         <v>0</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34"/>
-      <c r="L15" s="35"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32">
+        <v>1019</v>
+      </c>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="33"/>
     </row>
     <row r="16" spans="1:15" ht="20" thickBot="1">
-      <c r="A16" s="28">
+      <c r="A16" s="26">
         <v>1022</v>
       </c>
-      <c r="B16" s="28">
+      <c r="B16" s="26">
         <v>4</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="29">
-        <v>0</v>
-      </c>
-      <c r="F16" s="36" t="s">
+      <c r="D16" s="27">
+        <v>0</v>
+      </c>
+      <c r="F16" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="37">
+      <c r="G16" s="35">
         <v>24</v>
       </c>
-      <c r="H16" s="37">
+      <c r="H16" s="35">
         <f>G16-18</f>
         <v>6</v>
       </c>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
-      <c r="L16" s="38"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="36"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="28">
+      <c r="A17" s="26">
         <v>1028</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="26">
         <v>6</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="29">
-        <v>0</v>
-      </c>
-      <c r="E17" s="30" t="s">
+      <c r="D17" s="27">
+        <v>0</v>
+      </c>
+      <c r="E17" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F17" s="39"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40" t="s">
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38">
+        <v>1025</v>
+      </c>
+      <c r="I17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
+    </row>
+    <row r="18" spans="1:12" ht="20" thickBot="1">
+      <c r="A18" s="26">
+        <v>1011</v>
+      </c>
+      <c r="B18" s="26">
+        <v>7</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="27">
+        <v>0</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="35">
+        <v>24</v>
+      </c>
+      <c r="H18" s="35">
+        <f>G18-17</f>
+        <v>7</v>
+      </c>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="36"/>
+    </row>
+    <row r="19" spans="1:12" s="15" customFormat="1">
+      <c r="A19" s="29">
+        <v>1007</v>
+      </c>
+      <c r="B19" s="29">
+        <v>8</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="30">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I19" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+    </row>
+    <row r="20" spans="1:12" ht="20" thickBot="1">
+      <c r="A20" s="26">
+        <v>1008</v>
+      </c>
+      <c r="B20" s="26">
+        <v>16</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="27">
+        <v>0</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" s="35">
+        <v>8</v>
+      </c>
+      <c r="H20" s="35">
+        <f>G20-1</f>
+        <v>7</v>
+      </c>
+      <c r="I20" s="35">
+        <f>H20-6</f>
+        <v>1</v>
+      </c>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="36"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="29">
+        <v>1030</v>
+      </c>
+      <c r="B21" s="29">
+        <v>5</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="30">
+        <v>0</v>
+      </c>
+      <c r="F21" s="37"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+      <c r="J21" s="32"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="33"/>
+    </row>
+    <row r="22" spans="1:12" ht="20" thickBot="1">
+      <c r="A22" s="26">
+        <v>1005</v>
+      </c>
+      <c r="B22" s="26">
+        <v>16</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="27">
+        <v>0</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="35">
+        <v>8</v>
+      </c>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="36"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="26">
+        <v>1018</v>
+      </c>
+      <c r="B23" s="26">
+        <v>14</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="40" t="s">
-        <v>45</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="40" t="s">
-        <v>10</v>
-      </c>
-      <c r="L17" s="41"/>
-    </row>
-    <row r="18" spans="1:12" ht="20" thickBot="1">
-      <c r="A18" s="28">
-        <v>1011</v>
-      </c>
-      <c r="B18" s="28">
+      <c r="D23" s="27">
+        <v>0</v>
+      </c>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="33"/>
+    </row>
+    <row r="24" spans="1:12" ht="20" thickBot="1">
+      <c r="A24" s="26">
+        <v>1027</v>
+      </c>
+      <c r="B24" s="26">
+        <v>11</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="27">
+        <v>0</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="35">
+        <v>8</v>
+      </c>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="36"/>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="26">
+        <v>1023</v>
+      </c>
+      <c r="B25" s="26">
         <v>7</v>
       </c>
-      <c r="C18" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="29">
-        <v>0</v>
-      </c>
-      <c r="F18" s="36" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="37">
-        <v>24</v>
-      </c>
-      <c r="H18" s="37">
-        <f>G18-14</f>
-        <v>10</v>
-      </c>
-      <c r="I18" s="37">
-        <f>H18-6</f>
+      <c r="C25" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="27">
+        <v>0</v>
+      </c>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="K25" s="32"/>
+      <c r="L25" s="33"/>
+    </row>
+    <row r="26" spans="1:12" ht="20" thickBot="1">
+      <c r="A26" s="26">
+        <v>1024</v>
+      </c>
+      <c r="B26" s="26">
+        <v>13</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="27">
+        <v>0</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="35">
+        <v>8</v>
+      </c>
+      <c r="H26" s="35">
+        <f>G26-3</f>
+        <v>5</v>
+      </c>
+      <c r="I26" s="35">
+        <f>H26-1</f>
         <v>4</v>
       </c>
-      <c r="J18" s="37">
-        <f>HUC_Status!I18-2</f>
-        <v>2</v>
-      </c>
-      <c r="K18" s="37">
-        <f>J18-1</f>
-        <v>1</v>
-      </c>
-      <c r="L18" s="38"/>
-    </row>
-    <row r="19" spans="1:12" s="15" customFormat="1">
-      <c r="A19" s="31">
-        <v>1007</v>
-      </c>
-      <c r="B19" s="31">
-        <v>8</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="32">
-        <v>0</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="35"/>
-    </row>
-    <row r="20" spans="1:12" ht="20" thickBot="1">
-      <c r="A20" s="28">
-        <v>1008</v>
-      </c>
-      <c r="B20" s="28">
-        <v>16</v>
-      </c>
-      <c r="C20" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="29">
-        <v>0</v>
-      </c>
-      <c r="F20" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="G20" s="37">
-        <v>8</v>
-      </c>
-      <c r="H20" s="37">
-        <f>G20-8</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="38"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="31">
-        <v>1030</v>
-      </c>
-      <c r="B21" s="31">
-        <v>5</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="32">
-        <v>0</v>
-      </c>
-      <c r="F21" s="39"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>74</v>
-      </c>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="35"/>
-    </row>
-    <row r="22" spans="1:12" ht="20" thickBot="1">
-      <c r="A22" s="44">
-        <v>1005</v>
-      </c>
-      <c r="B22" s="44">
-        <v>16</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" s="37">
-        <v>8</v>
-      </c>
-      <c r="H22" s="37">
-        <f>G22-5</f>
+      <c r="J26" s="35">
+        <f>I26-1</f>
         <v>3</v>
       </c>
-      <c r="I22" s="37">
-        <f>H22-3</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="38"/>
-    </row>
-    <row r="23" spans="1:12">
-      <c r="A23" s="17">
-        <v>1018</v>
-      </c>
-      <c r="B23" s="17">
-        <v>14</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="35"/>
-    </row>
-    <row r="24" spans="1:12" ht="20" thickBot="1">
-      <c r="A24" s="17">
-        <v>1027</v>
-      </c>
-      <c r="B24" s="17">
-        <v>11</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="F24" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="37">
-        <v>8</v>
-      </c>
-      <c r="H24" s="37">
-        <f>G24-8</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="38"/>
-    </row>
-    <row r="25" spans="1:12">
-      <c r="A25" s="17">
-        <v>1023</v>
-      </c>
-      <c r="B25" s="17">
-        <v>7</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="40"/>
-      <c r="H25" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="35"/>
-    </row>
-    <row r="26" spans="1:12" ht="20" thickBot="1">
-      <c r="A26" s="17">
-        <v>1024</v>
-      </c>
-      <c r="B26" s="17">
-        <v>13</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="F26" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="37">
-        <v>8</v>
-      </c>
-      <c r="H26" s="37">
-        <f>G26-5</f>
-        <v>3</v>
-      </c>
-      <c r="I26" s="37">
-        <f>H26-3</f>
-        <v>0</v>
-      </c>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="38"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="36"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="44">
@@ -2649,41 +2638,43 @@
         <v>19</v>
       </c>
       <c r="E27" s="15"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="I27" s="34"/>
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="35"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="33"/>
     </row>
     <row r="28" spans="1:12" ht="20" thickBot="1">
-      <c r="A28" s="14">
+      <c r="A28" s="46">
         <v>1025</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="46">
         <v>17</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="13"/>
-      <c r="F28" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G28" s="37">
+      <c r="D28" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="35">
         <v>8</v>
       </c>
-      <c r="H28" s="37">
-        <f>G28-8</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
-      <c r="K28" s="37"/>
-      <c r="L28" s="38"/>
+      <c r="H28" s="35">
+        <f>G28-7</f>
+        <v>1</v>
+      </c>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35"/>
+      <c r="L28" s="36"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="14">
@@ -2696,15 +2687,17 @@
         <v>36</v>
       </c>
       <c r="D29" s="13"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="I29" s="34"/>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
-      <c r="L29" s="35"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="33"/>
     </row>
     <row r="30" spans="1:12" ht="20" thickBot="1">
       <c r="A30" s="14">
@@ -2717,20 +2710,23 @@
         <v>34</v>
       </c>
       <c r="D30" s="13"/>
-      <c r="F30" s="36" t="s">
+      <c r="F30" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="G30" s="37">
+      <c r="G30" s="35">
         <v>8</v>
       </c>
-      <c r="H30" s="37">
-        <f>G30-7</f>
+      <c r="H30" s="35">
+        <f>G30-1</f>
+        <v>7</v>
+      </c>
+      <c r="I30" s="35">
+        <f>H30-6</f>
         <v>1</v>
       </c>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
-      <c r="L30" s="38"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="36"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{67E277EF-276B-BB45-8B38-F26333CD85FF}">

</xml_diff>